<commit_message>
Finished keycodeConverter, started ALU stuff
Starting with the more complicated operations first, I implemented an integer square root algorithm.
</commit_message>
<xml_diff>
--- a/Keycodes.xlsx
+++ b/Keycodes.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elilo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57540F6C-A68C-4DA6-B06B-01C04890CADB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F658726-C635-46FF-B829-5ED97129CDAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14895" yWindow="840" windowWidth="22275" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9915" yWindow="1995" windowWidth="22275" windowHeight="14970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="172">
   <si>
     <t>Key</t>
   </si>
@@ -536,6 +535,12 @@
   </si>
   <si>
     <t>KP .</t>
+  </si>
+  <si>
+    <t>0x59</t>
+  </si>
+  <si>
+    <t>KP /</t>
   </si>
 </sst>
 </file>
@@ -867,7 +872,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,6 +1230,12 @@
         <v>117</v>
       </c>
       <c r="F16" s="1"/>
+      <c r="G16" t="s">
+        <v>170</v>
+      </c>
+      <c r="H16" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">

</xml_diff>